<commit_message>
fixed bug with place display and added regex mask to parse game results ina more flexible way
</commit_message>
<xml_diff>
--- a/Turnir2023.xlsx
+++ b/Turnir2023.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Шахматы" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="75">
   <si>
     <t xml:space="preserve">Айнура</t>
   </si>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">3:3</t>
   </si>
   <si>
-    <t xml:space="preserve">100:100</t>
+    <t xml:space="preserve">1.5:0.5</t>
   </si>
   <si>
     <t xml:space="preserve">14:0</t>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">3:1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5:1.5</t>
   </si>
   <si>
     <t xml:space="preserve">4:2</t>
@@ -487,11 +490,11 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -702,7 +705,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -729,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>35</v>
@@ -768,7 +771,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
@@ -908,16 +911,16 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5"/>
       <c r="D1" s="5"/>
@@ -946,27 +949,27 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -988,11 +991,11 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
@@ -1005,7 +1008,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>26</v>
@@ -1030,11 +1033,11 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>37</v>
@@ -1044,7 +1047,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>27</v>
@@ -1072,21 +1075,21 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>24</v>
@@ -1114,24 +1117,24 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>26</v>
@@ -1158,10 +1161,10 @@
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>27</v>
@@ -1170,7 +1173,7 @@
         <v>24</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="7" t="s">
@@ -1198,7 +1201,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>11</v>
@@ -29027,11 +29030,11 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -29039,7 +29042,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -29048,22 +29051,22 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29085,7 +29088,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -29132,7 +29135,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -29149,7 +29152,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -29166,7 +29169,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -29198,7 +29201,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -29215,7 +29218,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -29250,24 +29253,24 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -29276,19 +29279,19 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -29306,7 +29309,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="1"/>
@@ -29366,7 +29369,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -29426,7 +29429,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -29516,7 +29519,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -29546,7 +29549,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -29576,7 +29579,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -29606,7 +29609,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -29636,7 +29639,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>